<commit_message>
download added to messy. folders
folders created. for woody and wetland....
</commit_message>
<xml_diff>
--- a/MobileApi/DataFolder/Copy of Plant Database Woody.xlsx
+++ b/MobileApi/DataFolder/Copy of Plant Database Woody.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Marks Files\Natural Resources PRU\Apps\Woody Plants\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugene\Documents\GitHub\TestingMobileApi201810011322\MobileApi\DataFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8317733-C659-448F-8FF1-E27ECF7DF7FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -5522,7 +5521,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5616,7 +5615,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1" xfId="1"/>
+    <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5707,6 +5706,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5742,6 +5758,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5917,16 +5950,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CH150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="255.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="19.28515625" style="5"/>
+    <col min="1" max="1" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="29" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="93.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="52.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="164" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="238.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="62.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="38.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="132.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="58.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="47.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="53" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="49" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="234.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="228.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="138.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="60.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="113.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="84.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="241.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="55.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="235.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="130.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="98.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="237" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="235.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="52.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="142.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="46.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="104.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="39.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="123.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="72.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="235.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="26.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="87" max="16384" width="255.5703125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:86" x14ac:dyDescent="0.25">
@@ -6189,7 +6307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:86" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1039</v>
       </c>
@@ -6447,7 +6565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>593</v>
       </c>
@@ -6707,7 +6825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>184</v>
       </c>
@@ -6963,7 +7081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>308</v>
       </c>
@@ -7219,7 +7337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>188</v>
       </c>
@@ -7475,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>57</v>
       </c>
@@ -7733,7 +7851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>187</v>
       </c>
@@ -7991,7 +8109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>247</v>
       </c>
@@ -8251,7 +8369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>248</v>
       </c>
@@ -8507,7 +8625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:86" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1104</v>
       </c>
@@ -8763,7 +8881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>418</v>
       </c>
@@ -9019,7 +9137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>413</v>
       </c>
@@ -9277,7 +9395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>417</v>
       </c>
@@ -9533,7 +9651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:86" ht="195" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>371</v>
       </c>
@@ -9791,7 +9909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>310</v>
       </c>
@@ -10047,7 +10165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -10303,7 +10421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1102</v>
       </c>
@@ -10559,7 +10677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>511</v>
       </c>
@@ -10819,7 +10937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:86" ht="150" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>865</v>
       </c>
@@ -11075,7 +11193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>862</v>
       </c>
@@ -11331,7 +11449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:86" ht="255" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>864</v>
       </c>
@@ -11591,7 +11709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>863</v>
       </c>
@@ -11849,7 +11967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:86" ht="180" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>99</v>
       </c>
@@ -12105,7 +12223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:86" ht="195" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>259</v>
       </c>
@@ -12361,7 +12479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:86" ht="150" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>956</v>
       </c>
@@ -12617,7 +12735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1008</v>
       </c>
@@ -12873,7 +12991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:86" ht="165" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>249</v>
       </c>
@@ -13129,7 +13247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:86" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>380</v>
       </c>
@@ -13387,7 +13505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>214</v>
       </c>
@@ -13643,7 +13761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>838</v>
       </c>
@@ -13899,7 +14017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>836</v>
       </c>
@@ -14157,7 +14275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>839</v>
       </c>
@@ -14415,7 +14533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>841</v>
       </c>
@@ -14671,7 +14789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>835</v>
       </c>
@@ -14927,7 +15045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:86" ht="165" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>840</v>
       </c>
@@ -15183,7 +15301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>837</v>
       </c>
@@ -15441,7 +15559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>843</v>
       </c>
@@ -15697,7 +15815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>174</v>
       </c>
@@ -15957,7 +16075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>177</v>
       </c>
@@ -16213,7 +16331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:86" ht="90" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>884</v>
       </c>
@@ -16471,7 +16589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>176</v>
       </c>
@@ -16727,7 +16845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>175</v>
       </c>
@@ -16983,7 +17101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>513</v>
       </c>
@@ -17241,7 +17359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>1010</v>
       </c>
@@ -17497,7 +17615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>1134</v>
       </c>
@@ -17757,7 +17875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>1108</v>
       </c>
@@ -18013,7 +18131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>1011</v>
       </c>
@@ -18271,7 +18389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>880</v>
       </c>
@@ -18527,7 +18645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>881</v>
       </c>
@@ -18785,7 +18903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>1069</v>
       </c>
@@ -19043,7 +19161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>958</v>
       </c>
@@ -19303,7 +19421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>1063</v>
       </c>
@@ -19561,7 +19679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>357</v>
       </c>
@@ -19821,7 +19939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>957</v>
       </c>
@@ -20079,7 +20197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>502</v>
       </c>
@@ -20337,7 +20455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:86" ht="75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>1098</v>
       </c>
@@ -20593,7 +20711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>628</v>
       </c>
@@ -20851,7 +20969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>24</v>
       </c>
@@ -21111,7 +21229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:86" ht="180" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>581</v>
       </c>
@@ -21367,7 +21485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>822</v>
       </c>
@@ -21627,7 +21745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:86" ht="90" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>1103</v>
       </c>
@@ -21883,7 +22001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>914</v>
       </c>
@@ -22139,7 +22257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>374</v>
       </c>
@@ -22395,7 +22513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>913</v>
       </c>
@@ -22651,7 +22769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:86" ht="165" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>445</v>
       </c>
@@ -22907,7 +23025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:86" ht="180" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>845</v>
       </c>
@@ -23163,7 +23281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>73</v>
       </c>
@@ -23419,7 +23537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:86" ht="150" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>844</v>
       </c>
@@ -23679,7 +23797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>543</v>
       </c>
@@ -23935,7 +24053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>544</v>
       </c>
@@ -24191,7 +24309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:86" ht="150" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>758</v>
       </c>
@@ -24447,7 +24565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>756</v>
       </c>
@@ -24705,7 +24823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:86" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>1097</v>
       </c>
@@ -24961,7 +25079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>809</v>
       </c>
@@ -25219,7 +25337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:86" ht="165" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>755</v>
       </c>
@@ -25475,7 +25593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:86" ht="150" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>761</v>
       </c>
@@ -25731,7 +25849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:86" ht="165" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>759</v>
       </c>
@@ -25987,7 +26105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>763</v>
       </c>
@@ -26243,7 +26361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>760</v>
       </c>
@@ -26499,7 +26617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>762</v>
       </c>
@@ -26757,7 +26875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:86" ht="195" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>19</v>
       </c>
@@ -27015,7 +27133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>20</v>
       </c>
@@ -27273,7 +27391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>820</v>
       </c>
@@ -27529,7 +27647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:86" ht="165" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>437</v>
       </c>
@@ -27785,7 +27903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>596</v>
       </c>
@@ -28041,7 +28159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>847</v>
       </c>
@@ -28297,7 +28415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>656</v>
       </c>
@@ -28555,7 +28673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>688</v>
       </c>
@@ -28813,7 +28931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:86" ht="90" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>1099</v>
       </c>
@@ -29069,7 +29187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>312</v>
       </c>
@@ -29325,7 +29443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>939</v>
       </c>
@@ -29581,7 +29699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>365</v>
       </c>
@@ -29839,7 +29957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>257</v>
       </c>
@@ -30097,7 +30215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>253</v>
       </c>
@@ -30353,7 +30471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>311</v>
       </c>
@@ -30611,7 +30729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>313</v>
       </c>
@@ -30867,7 +30985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>497</v>
       </c>
@@ -31125,7 +31243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>754</v>
       </c>
@@ -31383,7 +31501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>254</v>
       </c>
@@ -31639,7 +31757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:86" ht="180" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>70</v>
       </c>
@@ -31897,7 +32015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>71</v>
       </c>
@@ -32153,7 +32271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>731</v>
       </c>
@@ -32411,7 +32529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>732</v>
       </c>
@@ -32667,7 +32785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:86" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>849</v>
       </c>
@@ -32923,7 +33041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>314</v>
       </c>
@@ -33179,7 +33297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:86" ht="195" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>805</v>
       </c>
@@ -33437,7 +33555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>850</v>
       </c>
@@ -33697,7 +33815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>848</v>
       </c>
@@ -33957,7 +34075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:86" ht="75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>5</v>
       </c>
@@ -34213,7 +34331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>698</v>
       </c>
@@ -34471,7 +34589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>988</v>
       </c>
@@ -34729,7 +34847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>834</v>
       </c>
@@ -34985,7 +35103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>833</v>
       </c>
@@ -35245,7 +35363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>909</v>
       </c>
@@ -35505,7 +35623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:86" ht="165" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>129</v>
       </c>
@@ -35763,7 +35881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>908</v>
       </c>
@@ -36021,7 +36139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>905</v>
       </c>
@@ -36279,7 +36397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>273</v>
       </c>
@@ -36539,7 +36657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>271</v>
       </c>
@@ -36795,7 +36913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:86" ht="195" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>275</v>
       </c>
@@ -37051,7 +37169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>1045</v>
       </c>
@@ -37307,7 +37425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:86" ht="120" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>1047</v>
       </c>
@@ -37565,7 +37683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>88</v>
       </c>
@@ -37823,7 +37941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:86" ht="255" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>910</v>
       </c>
@@ -38083,7 +38201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>550</v>
       </c>
@@ -38339,7 +38457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>648</v>
       </c>
@@ -38595,7 +38713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:86" ht="105" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>907</v>
       </c>
@@ -38851,7 +38969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>961</v>
       </c>
@@ -39107,7 +39225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:86" ht="255" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>960</v>
       </c>
@@ -39363,7 +39481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:86" ht="60" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>868</v>
       </c>
@@ -39621,7 +39739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>791</v>
       </c>
@@ -39879,7 +39997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>789</v>
       </c>
@@ -40135,7 +40253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:86" ht="90" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>1107</v>
       </c>
@@ -40391,7 +40509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>871</v>
       </c>
@@ -40649,7 +40767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>872</v>
       </c>
@@ -40905,7 +41023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>873</v>
       </c>
@@ -41161,7 +41279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:86" ht="240" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>792</v>
       </c>
@@ -41421,7 +41539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>874</v>
       </c>
@@ -41677,7 +41795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>788</v>
       </c>
@@ -41935,7 +42053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>867</v>
       </c>
@@ -42191,7 +42309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:86" ht="225" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>790</v>
       </c>
@@ -42449,7 +42567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:86" ht="90" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>875</v>
       </c>
@@ -42707,7 +42825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:86" ht="210" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>870</v>
       </c>
@@ -43223,7 +43341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:86" ht="60" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>869</v>
       </c>
@@ -43481,7 +43599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:86" ht="60" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>876</v>
       </c>
@@ -43739,7 +43857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>1177</v>
       </c>
@@ -43997,7 +44115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>1148</v>
       </c>
@@ -44255,7 +44373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:86" ht="135" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>12</v>
       </c>
@@ -44516,28 +44634,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>